<commit_message>
BraunEMEA Canada store(EN/FR) Stage code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/BraunEMEA/BraunUKTestData.xlsx
+++ b/src/test/resources/TestData/BraunEMEA/BraunUKTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B383C3-D6D8-4705-B191-9797A05434F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB52D082-174A-4436-9804-51D3C9A927C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22800" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22500" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="173">
   <si>
     <t>UserName</t>
   </si>
@@ -488,6 +488,57 @@
   </si>
   <si>
     <t>Hai aggiunto Braun ThermoScan® 7 con Age Precision® al tuo carrello.</t>
+  </si>
+  <si>
+    <t>CanadaENHearderlinks</t>
+  </si>
+  <si>
+    <t>CanadaHeaderlinks</t>
+  </si>
+  <si>
+    <t>Thermometers,Aspirators,Air Purifiers,Your Health</t>
+  </si>
+  <si>
+    <t>CanadaENNewsletter</t>
+  </si>
+  <si>
+    <t>CanadaNewsletter</t>
+  </si>
+  <si>
+    <t>Thank you for your subscription.</t>
+  </si>
+  <si>
+    <t>BabyRegistry</t>
+  </si>
+  <si>
+    <t>Building Your Baby Registry</t>
+  </si>
+  <si>
+    <t>CanadaProduct</t>
+  </si>
+  <si>
+    <t>ThermoScanᴹᴰ 5 avec ExacTemp</t>
+  </si>
+  <si>
+    <t>CanadaHeaderLinks</t>
+  </si>
+  <si>
+    <t>CanadaHeaders</t>
+  </si>
+  <si>
+    <t>Thermomètres,Nasaux,Purificateurs d’air,Votre santé</t>
+  </si>
+  <si>
+    <t>CanadaHealthlinkText</t>
+  </si>
+  <si>
+    <t>Créer votre registre de bébé</t>
+  </si>
+  <si>
+    <t>CanadahealthText</t>
+  </si>
+  <si>
+    <t>Combattre le rhume et la fièvre</t>
   </si>
 </sst>
 </file>
@@ -863,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA38"/>
+  <dimension ref="A1:BH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T26" sqref="T26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -882,24 +933,25 @@
     <col min="11" max="12" width="16" customWidth="1"/>
     <col min="16" max="16" width="28.85546875" customWidth="1"/>
     <col min="20" max="20" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="61" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="61" customWidth="1"/>
-    <col min="23" max="23" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="28" width="53.28515625" customWidth="1"/>
-    <col min="29" max="29" width="58.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="58.140625" customWidth="1"/>
-    <col min="31" max="31" width="60" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.140625" customWidth="1"/>
-    <col min="34" max="34" width="16" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="44" width="9.140625" style="5"/>
-    <col min="47" max="49" width="13.85546875" customWidth="1"/>
-    <col min="50" max="50" width="35.7109375" customWidth="1"/>
-    <col min="51" max="51" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="61.85546875" customWidth="1"/>
+    <col min="22" max="22" width="61" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="61" customWidth="1"/>
+    <col min="24" max="24" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="34" width="53.28515625" customWidth="1"/>
+    <col min="35" max="35" width="58.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="58.140625" customWidth="1"/>
+    <col min="38" max="38" width="60" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.140625" customWidth="1"/>
+    <col min="41" max="41" width="16" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="51" width="9.140625" style="5"/>
+    <col min="54" max="56" width="13.85546875" customWidth="1"/>
+    <col min="57" max="57" width="35.7109375" customWidth="1"/>
+    <col min="58" max="58" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53">
+    <row r="1" spans="1:60">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -961,104 +1013,125 @@
         <v>133</v>
       </c>
       <c r="U1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE1" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AI1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AK1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AQ1" s="2"/>
-      <c r="AR1" s="2" t="s">
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:53">
+    <row r="2" spans="1:60">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1080,12 +1153,12 @@
       <c r="G2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AO2"/>
-      <c r="AP2"/>
-      <c r="AQ2"/>
-      <c r="AR2"/>
-    </row>
-    <row r="3" spans="1:53">
+      <c r="AV2"/>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
+    </row>
+    <row r="3" spans="1:60">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1104,12 +1177,12 @@
       <c r="G3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AO3"/>
-      <c r="AP3"/>
-      <c r="AQ3"/>
-      <c r="AR3"/>
-    </row>
-    <row r="4" spans="1:53">
+      <c r="AV3"/>
+      <c r="AW3"/>
+      <c r="AX3"/>
+      <c r="AY3"/>
+    </row>
+    <row r="4" spans="1:60">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1142,12 +1215,12 @@
       <c r="N4" s="3">
         <v>9492846329</v>
       </c>
-      <c r="AO4"/>
-      <c r="AP4"/>
-      <c r="AQ4"/>
-      <c r="AR4"/>
-    </row>
-    <row r="5" spans="1:53">
+      <c r="AV4"/>
+      <c r="AW4"/>
+      <c r="AX4"/>
+      <c r="AY4"/>
+    </row>
+    <row r="5" spans="1:60">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1183,12 +1256,19 @@
       <c r="AF5" s="3"/>
       <c r="AG5" s="3"/>
       <c r="AH5" s="3"/>
-      <c r="AO5"/>
-      <c r="AP5"/>
-      <c r="AQ5"/>
-      <c r="AR5"/>
-    </row>
-    <row r="6" spans="1:53">
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
+      <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
+      <c r="AO5" s="3"/>
+      <c r="AV5"/>
+      <c r="AW5"/>
+      <c r="AX5"/>
+      <c r="AY5"/>
+    </row>
+    <row r="6" spans="1:60">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1224,12 +1304,19 @@
       <c r="AF6" s="3"/>
       <c r="AG6" s="3"/>
       <c r="AH6" s="3"/>
-      <c r="AO6"/>
-      <c r="AP6"/>
-      <c r="AQ6"/>
-      <c r="AR6"/>
-    </row>
-    <row r="7" spans="1:53">
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AV6"/>
+      <c r="AW6"/>
+      <c r="AX6"/>
+      <c r="AY6"/>
+    </row>
+    <row r="7" spans="1:60">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1237,24 +1324,24 @@
       <c r="D7" s="1"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
-      <c r="AI7" s="8" t="s">
+      <c r="AP7" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AQ7" t="s">
         <v>25</v>
       </c>
-      <c r="AK7" s="1" t="s">
+      <c r="AR7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AL7" s="1" t="s">
+      <c r="AS7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AO7"/>
-      <c r="AP7"/>
-      <c r="AQ7"/>
-      <c r="AR7"/>
-    </row>
-    <row r="8" spans="1:53">
+      <c r="AV7"/>
+      <c r="AW7"/>
+      <c r="AX7"/>
+      <c r="AY7"/>
+    </row>
+    <row r="8" spans="1:60">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1288,30 +1375,30 @@
       <c r="N8" s="3">
         <v>9898989899</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="AP8" t="s">
         <v>82</v>
       </c>
-      <c r="AJ8" t="s">
+      <c r="AQ8" t="s">
         <v>45</v>
       </c>
-      <c r="AM8">
+      <c r="AT8">
         <v>12341</v>
       </c>
-      <c r="AN8" t="s">
+      <c r="AU8" t="s">
         <v>44</v>
       </c>
-      <c r="AO8">
+      <c r="AV8">
         <v>5</v>
       </c>
-      <c r="AP8">
+      <c r="AW8">
         <v>6</v>
       </c>
-      <c r="AQ8"/>
-      <c r="AR8">
+      <c r="AX8"/>
+      <c r="AY8">
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="1:53">
+    <row r="9" spans="1:60">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1345,30 +1432,30 @@
       <c r="N9" s="3">
         <v>9898989899</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AP9" t="s">
         <v>82</v>
       </c>
-      <c r="AJ9" t="s">
+      <c r="AQ9" t="s">
         <v>45</v>
       </c>
-      <c r="AM9">
+      <c r="AT9">
         <v>12341</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AU9" t="s">
         <v>44</v>
       </c>
-      <c r="AO9">
+      <c r="AV9">
         <v>5</v>
       </c>
-      <c r="AP9">
+      <c r="AW9">
         <v>6</v>
       </c>
-      <c r="AQ9"/>
-      <c r="AR9">
+      <c r="AX9"/>
+      <c r="AY9">
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:53">
+    <row r="10" spans="1:60">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -1402,24 +1489,24 @@
       <c r="N10" s="3">
         <v>9898989899</v>
       </c>
-      <c r="AO10"/>
-      <c r="AP10"/>
-      <c r="AQ10"/>
-      <c r="AR10"/>
-    </row>
-    <row r="11" spans="1:53">
+      <c r="AV10"/>
+      <c r="AW10"/>
+      <c r="AX10"/>
+      <c r="AY10"/>
+    </row>
+    <row r="11" spans="1:60">
       <c r="A11" t="s">
         <v>52</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AP11" t="s">
         <v>53</v>
       </c>
-      <c r="AO11"/>
-      <c r="AP11"/>
-      <c r="AQ11"/>
-      <c r="AR11"/>
-    </row>
-    <row r="12" spans="1:53">
+      <c r="AV11"/>
+      <c r="AW11"/>
+      <c r="AX11"/>
+      <c r="AY11"/>
+    </row>
+    <row r="12" spans="1:60">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -1439,60 +1526,60 @@
       <c r="H12" t="s">
         <v>58</v>
       </c>
-      <c r="AO12"/>
-      <c r="AP12"/>
-      <c r="AQ12"/>
-      <c r="AR12"/>
-    </row>
-    <row r="13" spans="1:53">
+      <c r="AV12"/>
+      <c r="AW12"/>
+      <c r="AX12"/>
+      <c r="AY12"/>
+    </row>
+    <row r="13" spans="1:60">
       <c r="A13" t="s">
         <v>62</v>
       </c>
-      <c r="AI13" t="s">
+      <c r="AP13" t="s">
         <v>66</v>
       </c>
-      <c r="AO13"/>
-      <c r="AP13"/>
-      <c r="AQ13"/>
-      <c r="AR13"/>
-    </row>
-    <row r="14" spans="1:53">
+      <c r="AV13"/>
+      <c r="AW13"/>
+      <c r="AX13"/>
+      <c r="AY13"/>
+    </row>
+    <row r="14" spans="1:60">
       <c r="A14" t="s">
         <v>63</v>
       </c>
-      <c r="AI14" t="s">
+      <c r="AP14" t="s">
         <v>67</v>
       </c>
-      <c r="AO14"/>
-      <c r="AP14"/>
-      <c r="AQ14"/>
-      <c r="AR14"/>
-    </row>
-    <row r="15" spans="1:53">
+      <c r="AV14"/>
+      <c r="AW14"/>
+      <c r="AX14"/>
+      <c r="AY14"/>
+    </row>
+    <row r="15" spans="1:60">
       <c r="A15" t="s">
         <v>64</v>
       </c>
-      <c r="AI15" s="7" t="s">
+      <c r="AP15" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="AO15"/>
-      <c r="AP15"/>
-      <c r="AQ15"/>
-      <c r="AR15"/>
-    </row>
-    <row r="16" spans="1:53">
+      <c r="AV15"/>
+      <c r="AW15"/>
+      <c r="AX15"/>
+      <c r="AY15"/>
+    </row>
+    <row r="16" spans="1:60">
       <c r="A16" t="s">
         <v>65</v>
       </c>
-      <c r="AI16" s="7" t="s">
+      <c r="AP16" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AO16"/>
-      <c r="AP16"/>
-      <c r="AQ16"/>
-      <c r="AR16"/>
-    </row>
-    <row r="17" spans="1:53">
+      <c r="AV16"/>
+      <c r="AW16"/>
+      <c r="AX16"/>
+      <c r="AY16"/>
+    </row>
+    <row r="17" spans="1:60">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -1502,57 +1589,57 @@
       <c r="G17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AO17"/>
-      <c r="AP17"/>
-      <c r="AQ17"/>
-      <c r="AR17"/>
-      <c r="AS17" t="s">
+      <c r="AV17"/>
+      <c r="AW17"/>
+      <c r="AX17"/>
+      <c r="AY17"/>
+      <c r="AZ17" t="s">
         <v>28</v>
       </c>
-      <c r="AT17" t="s">
+      <c r="BA17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:53">
+    <row r="18" spans="1:60">
       <c r="A18" t="s">
         <v>75</v>
       </c>
-      <c r="AO18"/>
-      <c r="AP18"/>
-      <c r="AQ18"/>
-      <c r="AR18"/>
-      <c r="AZ18" t="s">
+      <c r="AV18"/>
+      <c r="AW18"/>
+      <c r="AX18"/>
+      <c r="AY18"/>
+      <c r="BG18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:53">
+    <row r="19" spans="1:60">
       <c r="A19" t="s">
         <v>78</v>
       </c>
-      <c r="AO19"/>
-      <c r="AP19"/>
-      <c r="AQ19"/>
-      <c r="AR19"/>
-      <c r="AZ19" t="s">
+      <c r="AV19"/>
+      <c r="AW19"/>
+      <c r="AX19"/>
+      <c r="AY19"/>
+      <c r="BG19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:53">
+    <row r="20" spans="1:60">
       <c r="A20" t="s">
         <v>80</v>
       </c>
-      <c r="AI20" t="s">
+      <c r="AP20" t="s">
         <v>81</v>
       </c>
-      <c r="AO20"/>
-      <c r="AP20"/>
-      <c r="AQ20"/>
-      <c r="AR20"/>
-      <c r="BA20" t="s">
+      <c r="AV20"/>
+      <c r="AW20"/>
+      <c r="AX20"/>
+      <c r="AY20"/>
+      <c r="BH20" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:53">
+    <row r="21" spans="1:60">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -1572,7 +1659,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:53">
+    <row r="22" spans="1:60">
       <c r="A22" t="s">
         <v>99</v>
       </c>
@@ -1601,12 +1688,19 @@
       <c r="AD22" s="7"/>
       <c r="AE22" s="7"/>
       <c r="AF22" s="7"/>
-      <c r="AG22" s="7" t="s">
+      <c r="AG22" s="7"/>
+      <c r="AH22" s="7"/>
+      <c r="AI22" s="7"/>
+      <c r="AJ22" s="7"/>
+      <c r="AK22" s="7"/>
+      <c r="AL22" s="7"/>
+      <c r="AM22" s="7"/>
+      <c r="AN22" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="AH22" s="7"/>
-    </row>
-    <row r="23" spans="1:53">
+      <c r="AO22" s="7"/>
+    </row>
+    <row r="23" spans="1:60">
       <c r="A23" t="s">
         <v>101</v>
       </c>
@@ -1635,7 +1729,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="24" spans="1:53">
+    <row r="24" spans="1:60">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1643,97 +1737,98 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:53">
+    <row r="25" spans="1:60">
       <c r="A25" t="s">
         <v>106</v>
       </c>
-      <c r="AY25" t="s">
+      <c r="BF25" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:53" ht="60">
+    <row r="26" spans="1:60" ht="60">
       <c r="A26" t="s">
         <v>109</v>
       </c>
-      <c r="AX26" s="10" t="s">
+      <c r="BE26" s="10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:53">
+    <row r="27" spans="1:60">
       <c r="A27" t="s">
         <v>112</v>
       </c>
-      <c r="AU27" s="11" t="s">
+      <c r="BB27" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="AV27" s="11"/>
-      <c r="AW27" s="11"/>
-    </row>
-    <row r="28" spans="1:53">
+      <c r="BC27" s="11"/>
+      <c r="BD27" s="11"/>
+    </row>
+    <row r="28" spans="1:60">
       <c r="A28" t="s">
         <v>115</v>
       </c>
-      <c r="AF28" t="s">
+      <c r="AM28" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:53">
+    <row r="29" spans="1:60">
       <c r="A29" t="s">
         <v>118</v>
       </c>
-      <c r="AW29" s="11" t="s">
+      <c r="BD29" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:53">
+    <row r="30" spans="1:60">
       <c r="A30" t="s">
         <v>121</v>
       </c>
-      <c r="AV30" s="12" t="s">
+      <c r="BC30" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:53">
+    <row r="31" spans="1:60">
       <c r="A31" t="s">
         <v>123</v>
       </c>
-      <c r="AE31" t="s">
+      <c r="AL31" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:53">
+    <row r="32" spans="1:60">
       <c r="A32" t="s">
         <v>126</v>
       </c>
-      <c r="W32" t="s">
+      <c r="X32" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:29">
+    <row r="33" spans="1:36">
       <c r="A33" t="s">
         <v>52</v>
       </c>
-      <c r="W33" t="s">
+      <c r="X33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:36">
       <c r="A34" t="s">
         <v>128</v>
       </c>
-      <c r="U34" t="s">
+      <c r="V34" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:36">
       <c r="A35" t="s">
         <v>131</v>
       </c>
       <c r="T35" s="13" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="36" spans="1:29">
+      <c r="U35" s="13"/>
+    </row>
+    <row r="36" spans="1:36">
       <c r="A36" t="s">
         <v>134</v>
       </c>
@@ -1741,43 +1836,84 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:29">
+    <row r="37" spans="1:36">
       <c r="A37" t="s">
         <v>136</v>
       </c>
-      <c r="X37" t="s">
+      <c r="Y37" t="s">
         <v>140</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>141</v>
       </c>
       <c r="Z37" t="s">
         <v>141</v>
       </c>
       <c r="AA37" t="s">
+        <v>163</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF37" t="s">
         <v>147</v>
       </c>
-      <c r="AB37" t="s">
+      <c r="AG37" t="s">
         <v>145</v>
       </c>
-      <c r="AC37" t="s">
+      <c r="AI37" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:29">
+    <row r="38" spans="1:36">
       <c r="A38" t="s">
         <v>149</v>
       </c>
-      <c r="V38" t="s">
+      <c r="W38" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36">
+      <c r="A39" t="s">
+        <v>156</v>
+      </c>
+      <c r="AH39" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36">
+      <c r="A40" t="s">
+        <v>159</v>
+      </c>
+      <c r="AJ40" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36">
+      <c r="A41" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36">
+      <c r="A42" t="s">
+        <v>166</v>
+      </c>
+      <c r="U42" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Vihaan@2018" xr:uid="{4F5DD53B-FDBE-495F-B268-88C5E8B1BE36}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{4B3C725C-3736-453A-973F-014EA407F106}"/>
-    <hyperlink ref="AK7" r:id="rId3" xr:uid="{72305042-87C7-4932-8AE0-68B10841BE88}"/>
-    <hyperlink ref="AL7" r:id="rId4" xr:uid="{475D0090-7A14-45A1-B12D-CC9A2AB68BA3}"/>
+    <hyperlink ref="AR7" r:id="rId3" xr:uid="{72305042-87C7-4932-8AE0-68B10841BE88}"/>
+    <hyperlink ref="AS7" r:id="rId4" xr:uid="{475D0090-7A14-45A1-B12D-CC9A2AB68BA3}"/>
     <hyperlink ref="G8" r:id="rId5" xr:uid="{01FC8DE1-D0EC-434A-A443-9B88FB015484}"/>
     <hyperlink ref="G9" r:id="rId6" xr:uid="{7F86A831-6BAE-4F74-AB10-D461CC901815}"/>
     <hyperlink ref="G10" r:id="rId7" xr:uid="{F135D05F-7B8D-4589-985B-77D2AC13D428}"/>

</xml_diff>

<commit_message>
BraunEMEA Italy and Sweden Stage code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/BraunEMEA/BraunUKTestData.xlsx
+++ b/src/test/resources/TestData/BraunEMEA/BraunUKTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB52D082-174A-4436-9804-51D3C9A927C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A216A9-7783-4A4D-B512-9D35D602E41E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="22500" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="193">
   <si>
     <t>UserName</t>
   </si>
@@ -539,6 +539,66 @@
   </si>
   <si>
     <t>Combattre le rhume et la fièvre</t>
+  </si>
+  <si>
+    <t>ItalyAccountDetails</t>
+  </si>
+  <si>
+    <t>ganeshnarra65@gmail.com</t>
+  </si>
+  <si>
+    <t>Ganesh@123</t>
+  </si>
+  <si>
+    <t>Ganesh</t>
+  </si>
+  <si>
+    <t>gani</t>
+  </si>
+  <si>
+    <t>ItalyLogin</t>
+  </si>
+  <si>
+    <t>Shipping_Address</t>
+  </si>
+  <si>
+    <t>rajkumar</t>
+  </si>
+  <si>
+    <t>RK</t>
+  </si>
+  <si>
+    <t>rajkumarpotharaju1997@gmail.com</t>
+  </si>
+  <si>
+    <t>SwedenProductname</t>
+  </si>
+  <si>
+    <t>Braun ThermoScan 5 with ExactTemp</t>
+  </si>
+  <si>
+    <t>ItalynewsletterSubscription</t>
+  </si>
+  <si>
+    <t>Grazie per l'iscrizione.</t>
+  </si>
+  <si>
+    <t>ItalyProductname</t>
+  </si>
+  <si>
+    <t>Italyproduct</t>
+  </si>
+  <si>
+    <t>Braun ThermoScan® 3</t>
+  </si>
+  <si>
+    <t>ITManageAddress</t>
+  </si>
+  <si>
+    <t>ITAddress</t>
+  </si>
+  <si>
+    <t>Rubrica</t>
   </si>
 </sst>
 </file>
@@ -914,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH42"/>
+  <dimension ref="A1:BL47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AK10" sqref="AK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -933,25 +993,25 @@
     <col min="11" max="12" width="16" customWidth="1"/>
     <col min="16" max="16" width="28.85546875" customWidth="1"/>
     <col min="20" max="20" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="61.85546875" customWidth="1"/>
-    <col min="22" max="22" width="61" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="61" customWidth="1"/>
-    <col min="24" max="24" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="34" width="53.28515625" customWidth="1"/>
-    <col min="35" max="35" width="58.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="58.140625" customWidth="1"/>
-    <col min="38" max="38" width="60" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.140625" customWidth="1"/>
-    <col min="41" max="41" width="16" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="51" width="9.140625" style="5"/>
-    <col min="54" max="56" width="13.85546875" customWidth="1"/>
-    <col min="57" max="57" width="35.7109375" customWidth="1"/>
-    <col min="58" max="58" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="61.85546875" customWidth="1"/>
+    <col min="23" max="23" width="61" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="61" customWidth="1"/>
+    <col min="25" max="25" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="36" width="53.28515625" customWidth="1"/>
+    <col min="37" max="37" width="58.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="41" width="58.140625" customWidth="1"/>
+    <col min="42" max="42" width="60" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.140625" customWidth="1"/>
+    <col min="45" max="45" width="16" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="52" max="55" width="9.140625" style="5"/>
+    <col min="58" max="60" width="13.85546875" customWidth="1"/>
+    <col min="61" max="61" width="35.7109375" customWidth="1"/>
+    <col min="62" max="62" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60">
+    <row r="1" spans="1:64">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1016,122 +1076,134 @@
         <v>167</v>
       </c>
       <c r="V1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC1" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="AM1" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AP1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="2"/>
-      <c r="AY1" s="2" t="s">
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:60">
+    <row r="2" spans="1:64">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1153,12 +1225,12 @@
       <c r="G2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AV2"/>
-      <c r="AW2"/>
-      <c r="AX2"/>
-      <c r="AY2"/>
-    </row>
-    <row r="3" spans="1:60">
+      <c r="AZ2"/>
+      <c r="BA2"/>
+      <c r="BB2"/>
+      <c r="BC2"/>
+    </row>
+    <row r="3" spans="1:64">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1177,12 +1249,12 @@
       <c r="G3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AV3"/>
-      <c r="AW3"/>
-      <c r="AX3"/>
-      <c r="AY3"/>
-    </row>
-    <row r="4" spans="1:60">
+      <c r="AZ3"/>
+      <c r="BA3"/>
+      <c r="BB3"/>
+      <c r="BC3"/>
+    </row>
+    <row r="4" spans="1:64">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1215,12 +1287,12 @@
       <c r="N4" s="3">
         <v>9492846329</v>
       </c>
-      <c r="AV4"/>
-      <c r="AW4"/>
-      <c r="AX4"/>
-      <c r="AY4"/>
-    </row>
-    <row r="5" spans="1:60">
+      <c r="AZ4"/>
+      <c r="BA4"/>
+      <c r="BB4"/>
+      <c r="BC4"/>
+    </row>
+    <row r="5" spans="1:64">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1263,12 +1335,16 @@
       <c r="AM5" s="3"/>
       <c r="AN5" s="3"/>
       <c r="AO5" s="3"/>
-      <c r="AV5"/>
-      <c r="AW5"/>
-      <c r="AX5"/>
-      <c r="AY5"/>
-    </row>
-    <row r="6" spans="1:60">
+      <c r="AP5" s="3"/>
+      <c r="AQ5" s="3"/>
+      <c r="AR5" s="3"/>
+      <c r="AS5" s="3"/>
+      <c r="AZ5"/>
+      <c r="BA5"/>
+      <c r="BB5"/>
+      <c r="BC5"/>
+    </row>
+    <row r="6" spans="1:64">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1311,12 +1387,16 @@
       <c r="AM6" s="3"/>
       <c r="AN6" s="3"/>
       <c r="AO6" s="3"/>
-      <c r="AV6"/>
-      <c r="AW6"/>
-      <c r="AX6"/>
-      <c r="AY6"/>
-    </row>
-    <row r="7" spans="1:60">
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AZ6"/>
+      <c r="BA6"/>
+      <c r="BB6"/>
+      <c r="BC6"/>
+    </row>
+    <row r="7" spans="1:64">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1324,24 +1404,27 @@
       <c r="D7" s="1"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
-      <c r="AP7" s="8" t="s">
+      <c r="AO7" t="s">
+        <v>184</v>
+      </c>
+      <c r="AT7" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="AQ7" t="s">
+      <c r="AU7" t="s">
         <v>25</v>
       </c>
-      <c r="AR7" s="1" t="s">
+      <c r="AV7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AS7" s="1" t="s">
+      <c r="AW7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AV7"/>
-      <c r="AW7"/>
-      <c r="AX7"/>
-      <c r="AY7"/>
-    </row>
-    <row r="8" spans="1:60">
+      <c r="AZ7"/>
+      <c r="BA7"/>
+      <c r="BB7"/>
+      <c r="BC7"/>
+    </row>
+    <row r="8" spans="1:64">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1375,30 +1458,30 @@
       <c r="N8" s="3">
         <v>9898989899</v>
       </c>
-      <c r="AP8" t="s">
+      <c r="AT8" t="s">
         <v>82</v>
       </c>
-      <c r="AQ8" t="s">
+      <c r="AU8" t="s">
         <v>45</v>
       </c>
-      <c r="AT8">
+      <c r="AX8">
         <v>12341</v>
       </c>
-      <c r="AU8" t="s">
+      <c r="AY8" t="s">
         <v>44</v>
       </c>
-      <c r="AV8">
+      <c r="AZ8">
         <v>5</v>
       </c>
-      <c r="AW8">
+      <c r="BA8">
         <v>6</v>
       </c>
-      <c r="AX8"/>
-      <c r="AY8">
+      <c r="BB8"/>
+      <c r="BC8">
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="1:60">
+    <row r="9" spans="1:64">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1432,30 +1515,30 @@
       <c r="N9" s="3">
         <v>9898989899</v>
       </c>
-      <c r="AP9" t="s">
+      <c r="AT9" t="s">
         <v>82</v>
       </c>
-      <c r="AQ9" t="s">
+      <c r="AU9" t="s">
         <v>45</v>
       </c>
-      <c r="AT9">
+      <c r="AX9">
         <v>12341</v>
       </c>
-      <c r="AU9" t="s">
+      <c r="AY9" t="s">
         <v>44</v>
       </c>
-      <c r="AV9">
+      <c r="AZ9">
         <v>5</v>
       </c>
-      <c r="AW9">
+      <c r="BA9">
         <v>6</v>
       </c>
-      <c r="AX9"/>
-      <c r="AY9">
+      <c r="BB9"/>
+      <c r="BC9">
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:60">
+    <row r="10" spans="1:64">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -1489,24 +1572,24 @@
       <c r="N10" s="3">
         <v>9898989899</v>
       </c>
-      <c r="AV10"/>
-      <c r="AW10"/>
-      <c r="AX10"/>
-      <c r="AY10"/>
-    </row>
-    <row r="11" spans="1:60">
+      <c r="AZ10"/>
+      <c r="BA10"/>
+      <c r="BB10"/>
+      <c r="BC10"/>
+    </row>
+    <row r="11" spans="1:64">
       <c r="A11" t="s">
         <v>52</v>
       </c>
-      <c r="AP11" t="s">
+      <c r="AT11" t="s">
         <v>53</v>
       </c>
-      <c r="AV11"/>
-      <c r="AW11"/>
-      <c r="AX11"/>
-      <c r="AY11"/>
-    </row>
-    <row r="12" spans="1:60">
+      <c r="AZ11"/>
+      <c r="BA11"/>
+      <c r="BB11"/>
+      <c r="BC11"/>
+    </row>
+    <row r="12" spans="1:64">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -1526,60 +1609,60 @@
       <c r="H12" t="s">
         <v>58</v>
       </c>
-      <c r="AV12"/>
-      <c r="AW12"/>
-      <c r="AX12"/>
-      <c r="AY12"/>
-    </row>
-    <row r="13" spans="1:60">
+      <c r="AZ12"/>
+      <c r="BA12"/>
+      <c r="BB12"/>
+      <c r="BC12"/>
+    </row>
+    <row r="13" spans="1:64">
       <c r="A13" t="s">
         <v>62</v>
       </c>
-      <c r="AP13" t="s">
+      <c r="AT13" t="s">
         <v>66</v>
       </c>
-      <c r="AV13"/>
-      <c r="AW13"/>
-      <c r="AX13"/>
-      <c r="AY13"/>
-    </row>
-    <row r="14" spans="1:60">
+      <c r="AZ13"/>
+      <c r="BA13"/>
+      <c r="BB13"/>
+      <c r="BC13"/>
+    </row>
+    <row r="14" spans="1:64">
       <c r="A14" t="s">
         <v>63</v>
       </c>
-      <c r="AP14" t="s">
+      <c r="AT14" t="s">
         <v>67</v>
       </c>
-      <c r="AV14"/>
-      <c r="AW14"/>
-      <c r="AX14"/>
-      <c r="AY14"/>
-    </row>
-    <row r="15" spans="1:60">
+      <c r="AZ14"/>
+      <c r="BA14"/>
+      <c r="BB14"/>
+      <c r="BC14"/>
+    </row>
+    <row r="15" spans="1:64">
       <c r="A15" t="s">
         <v>64</v>
       </c>
-      <c r="AP15" s="7" t="s">
+      <c r="AT15" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="AV15"/>
-      <c r="AW15"/>
-      <c r="AX15"/>
-      <c r="AY15"/>
-    </row>
-    <row r="16" spans="1:60">
+      <c r="AZ15"/>
+      <c r="BA15"/>
+      <c r="BB15"/>
+      <c r="BC15"/>
+    </row>
+    <row r="16" spans="1:64">
       <c r="A16" t="s">
         <v>65</v>
       </c>
-      <c r="AP16" s="7" t="s">
+      <c r="AT16" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AV16"/>
-      <c r="AW16"/>
-      <c r="AX16"/>
-      <c r="AY16"/>
-    </row>
-    <row r="17" spans="1:60">
+      <c r="AZ16"/>
+      <c r="BA16"/>
+      <c r="BB16"/>
+      <c r="BC16"/>
+    </row>
+    <row r="17" spans="1:64">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -1589,57 +1672,57 @@
       <c r="G17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AV17"/>
-      <c r="AW17"/>
-      <c r="AX17"/>
-      <c r="AY17"/>
-      <c r="AZ17" t="s">
+      <c r="AZ17"/>
+      <c r="BA17"/>
+      <c r="BB17"/>
+      <c r="BC17"/>
+      <c r="BD17" t="s">
         <v>28</v>
       </c>
-      <c r="BA17" t="s">
+      <c r="BE17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:60">
+    <row r="18" spans="1:64">
       <c r="A18" t="s">
         <v>75</v>
       </c>
-      <c r="AV18"/>
-      <c r="AW18"/>
-      <c r="AX18"/>
-      <c r="AY18"/>
-      <c r="BG18" t="s">
+      <c r="AZ18"/>
+      <c r="BA18"/>
+      <c r="BB18"/>
+      <c r="BC18"/>
+      <c r="BK18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:60">
+    <row r="19" spans="1:64">
       <c r="A19" t="s">
         <v>78</v>
       </c>
-      <c r="AV19"/>
-      <c r="AW19"/>
-      <c r="AX19"/>
-      <c r="AY19"/>
-      <c r="BG19" t="s">
+      <c r="AZ19"/>
+      <c r="BA19"/>
+      <c r="BB19"/>
+      <c r="BC19"/>
+      <c r="BK19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:60">
+    <row r="20" spans="1:64">
       <c r="A20" t="s">
         <v>80</v>
       </c>
-      <c r="AP20" t="s">
+      <c r="AT20" t="s">
         <v>81</v>
       </c>
-      <c r="AV20"/>
-      <c r="AW20"/>
-      <c r="AX20"/>
-      <c r="AY20"/>
-      <c r="BH20" t="s">
+      <c r="AZ20"/>
+      <c r="BA20"/>
+      <c r="BB20"/>
+      <c r="BC20"/>
+      <c r="BL20" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:60">
+    <row r="21" spans="1:64">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -1659,7 +1742,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:60">
+    <row r="22" spans="1:64">
       <c r="A22" t="s">
         <v>99</v>
       </c>
@@ -1695,12 +1778,16 @@
       <c r="AK22" s="7"/>
       <c r="AL22" s="7"/>
       <c r="AM22" s="7"/>
-      <c r="AN22" s="7" t="s">
+      <c r="AN22" s="7"/>
+      <c r="AO22" s="7"/>
+      <c r="AP22" s="7"/>
+      <c r="AQ22" s="7"/>
+      <c r="AR22" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="AO22" s="7"/>
-    </row>
-    <row r="23" spans="1:60">
+      <c r="AS22" s="7"/>
+    </row>
+    <row r="23" spans="1:64">
       <c r="A23" t="s">
         <v>101</v>
       </c>
@@ -1729,7 +1816,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="24" spans="1:60">
+    <row r="24" spans="1:64">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1737,89 +1824,89 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:60">
+    <row r="25" spans="1:64">
       <c r="A25" t="s">
         <v>106</v>
       </c>
-      <c r="BF25" t="s">
+      <c r="BJ25" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:60" ht="60">
+    <row r="26" spans="1:64" ht="60">
       <c r="A26" t="s">
         <v>109</v>
       </c>
-      <c r="BE26" s="10" t="s">
+      <c r="BI26" s="10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:60">
+    <row r="27" spans="1:64">
       <c r="A27" t="s">
         <v>112</v>
       </c>
-      <c r="BB27" s="11" t="s">
+      <c r="BF27" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="BC27" s="11"/>
-      <c r="BD27" s="11"/>
-    </row>
-    <row r="28" spans="1:60">
+      <c r="BG27" s="11"/>
+      <c r="BH27" s="11"/>
+    </row>
+    <row r="28" spans="1:64">
       <c r="A28" t="s">
         <v>115</v>
       </c>
-      <c r="AM28" t="s">
+      <c r="AQ28" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:60">
+    <row r="29" spans="1:64">
       <c r="A29" t="s">
         <v>118</v>
       </c>
-      <c r="BD29" s="11" t="s">
+      <c r="BH29" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:60">
+    <row r="30" spans="1:64">
       <c r="A30" t="s">
         <v>121</v>
       </c>
-      <c r="BC30" s="12" t="s">
+      <c r="BG30" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:60">
+    <row r="31" spans="1:64">
       <c r="A31" t="s">
         <v>123</v>
       </c>
-      <c r="AL31" t="s">
+      <c r="AP31" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:60">
+    <row r="32" spans="1:64">
       <c r="A32" t="s">
         <v>126</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Y32" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:36">
+    <row r="33" spans="1:39">
       <c r="A33" t="s">
         <v>52</v>
       </c>
-      <c r="X33" t="s">
+      <c r="Y33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:36">
+    <row r="34" spans="1:39">
       <c r="A34" t="s">
         <v>128</v>
       </c>
-      <c r="V34" t="s">
+      <c r="W34" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:36">
+    <row r="35" spans="1:39">
       <c r="A35" t="s">
         <v>131</v>
       </c>
@@ -1827,8 +1914,12 @@
         <v>155</v>
       </c>
       <c r="U35" s="13"/>
-    </row>
-    <row r="36" spans="1:36">
+      <c r="V35" s="13"/>
+      <c r="AB35" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39">
       <c r="A36" t="s">
         <v>134</v>
       </c>
@@ -1836,84 +1927,163 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:36">
+    <row r="37" spans="1:39">
       <c r="A37" t="s">
         <v>136</v>
       </c>
-      <c r="Y37" t="s">
+      <c r="Z37" t="s">
         <v>140</v>
       </c>
-      <c r="Z37" t="s">
+      <c r="AA37" t="s">
         <v>141</v>
       </c>
-      <c r="AA37" t="s">
+      <c r="AC37" t="s">
         <v>163</v>
       </c>
-      <c r="AC37" t="s">
+      <c r="AE37" t="s">
         <v>172</v>
       </c>
-      <c r="AD37" t="s">
+      <c r="AF37" t="s">
         <v>170</v>
       </c>
-      <c r="AE37" t="s">
+      <c r="AG37" t="s">
         <v>141</v>
       </c>
-      <c r="AF37" t="s">
+      <c r="AH37" t="s">
         <v>147</v>
       </c>
-      <c r="AG37" t="s">
+      <c r="AI37" t="s">
         <v>145</v>
       </c>
-      <c r="AI37" t="s">
+      <c r="AK37" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:36">
+    <row r="38" spans="1:39">
       <c r="A38" t="s">
         <v>149</v>
       </c>
-      <c r="W38" t="s">
+      <c r="X38" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:36">
+    <row r="39" spans="1:39">
       <c r="A39" t="s">
         <v>156</v>
       </c>
-      <c r="AH39" t="s">
+      <c r="AJ39" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="40" spans="1:36">
+    <row r="40" spans="1:39">
       <c r="A40" t="s">
         <v>159</v>
       </c>
-      <c r="AJ40" t="s">
+      <c r="AM40" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="41" spans="1:36">
+    <row r="41" spans="1:39">
       <c r="A41" t="s">
         <v>164</v>
       </c>
-      <c r="AB41" t="s">
+      <c r="AD41" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:36">
+    <row r="42" spans="1:39">
       <c r="A42" t="s">
         <v>166</v>
       </c>
       <c r="U42" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39">
+      <c r="A43" t="s">
+        <v>173</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E43" t="s">
+        <v>176</v>
+      </c>
+      <c r="F43" t="s">
+        <v>177</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39">
+      <c r="A44" t="s">
+        <v>178</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:39">
+      <c r="A45" t="s">
+        <v>179</v>
+      </c>
+      <c r="E45" t="s">
+        <v>180</v>
+      </c>
+      <c r="F45" t="s">
+        <v>181</v>
+      </c>
+      <c r="G45" t="s">
+        <v>182</v>
+      </c>
+      <c r="H45" t="s">
+        <v>33</v>
+      </c>
+      <c r="K45" t="s">
+        <v>35</v>
+      </c>
+      <c r="M45">
+        <v>12345</v>
+      </c>
+      <c r="N45">
+        <v>9492846329</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39">
+      <c r="A46" t="s">
+        <v>187</v>
+      </c>
+      <c r="V46" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39">
+      <c r="A47" t="s">
+        <v>190</v>
+      </c>
+      <c r="AL47" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Vihaan@2018" xr:uid="{4F5DD53B-FDBE-495F-B268-88C5E8B1BE36}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{4B3C725C-3736-453A-973F-014EA407F106}"/>
-    <hyperlink ref="AR7" r:id="rId3" xr:uid="{72305042-87C7-4932-8AE0-68B10841BE88}"/>
-    <hyperlink ref="AS7" r:id="rId4" xr:uid="{475D0090-7A14-45A1-B12D-CC9A2AB68BA3}"/>
+    <hyperlink ref="AV7" r:id="rId3" xr:uid="{72305042-87C7-4932-8AE0-68B10841BE88}"/>
+    <hyperlink ref="AW7" r:id="rId4" xr:uid="{475D0090-7A14-45A1-B12D-CC9A2AB68BA3}"/>
     <hyperlink ref="G8" r:id="rId5" xr:uid="{01FC8DE1-D0EC-434A-A443-9B88FB015484}"/>
     <hyperlink ref="G9" r:id="rId6" xr:uid="{7F86A831-6BAE-4F74-AB10-D461CC901815}"/>
     <hyperlink ref="G10" r:id="rId7" xr:uid="{F135D05F-7B8D-4589-985B-77D2AC13D428}"/>
@@ -1928,8 +2098,15 @@
     <hyperlink ref="D2" r:id="rId16" display="Vihaan@2018" xr:uid="{5C518423-99A0-4586-B3F5-D544A737B8F9}"/>
     <hyperlink ref="G23" r:id="rId17" xr:uid="{1271EC5C-450C-4B58-9AE6-69B21901206E}"/>
     <hyperlink ref="G24" r:id="rId18" xr:uid="{4C9855DC-6136-4EC1-B891-FB67685B8484}"/>
+    <hyperlink ref="B43" r:id="rId19" xr:uid="{E6B3FA17-5B57-4416-BDD3-91CF4EEC85D0}"/>
+    <hyperlink ref="C43" r:id="rId20" xr:uid="{E64F5A25-4DA8-46BD-838F-574B6DB05927}"/>
+    <hyperlink ref="D43" r:id="rId21" xr:uid="{C9748A95-B1CA-47DF-AA51-00A799A5CA31}"/>
+    <hyperlink ref="B44" r:id="rId22" xr:uid="{1E3AF817-4B8E-42D4-8F7B-0BCE2E35316F}"/>
+    <hyperlink ref="C44" r:id="rId23" xr:uid="{03AE5693-B809-440D-AFF6-4E56A33D210F}"/>
+    <hyperlink ref="G43" r:id="rId24" xr:uid="{B7F7FE31-A565-423F-9484-A0BBD29B1DAE}"/>
+    <hyperlink ref="G44" r:id="rId25" xr:uid="{8743381F-49E5-42D0-846F-4FD5EA879AED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId19"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Braun EMEA updated code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/BraunEMEA/BraunUKTestData.xlsx
+++ b/src/test/resources/TestData/BraunEMEA/BraunUKTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2390B605-6877-40DF-AF5A-FB7BA965E79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF238213-5B6F-4CC9-9DE5-A3FA9EE124F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22800" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="213">
   <si>
     <t>UserName</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Chiruvella</t>
   </si>
   <si>
-    <t>harish.chiruvella1@gmail.com</t>
-  </si>
-  <si>
     <t>productName</t>
   </si>
   <si>
@@ -328,9 +325,6 @@
     <t>GuestEmail</t>
   </si>
   <si>
-    <t>sathyamjothi2622@gmail.com</t>
-  </si>
-  <si>
     <t>pranaya</t>
   </si>
   <si>
@@ -635,6 +629,36 @@
   </si>
   <si>
     <t>Braun ThermoScan® 7 avec Age Precision®</t>
+  </si>
+  <si>
+    <t>rajkumarpotharaju1995@gmail.com</t>
+  </si>
+  <si>
+    <t>123456789@Raju</t>
+  </si>
+  <si>
+    <t>ganesh123@gmail.com</t>
+  </si>
+  <si>
+    <t>socalLinks</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Facebook,Instagram,Youtube</t>
+  </si>
+  <si>
+    <t>3DCardDetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4917610000000000	</t>
+  </si>
+  <si>
+    <t>3DPassword</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -1010,44 +1034,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BN50"/>
+  <dimension ref="A1:BO53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32" customWidth="1"/>
+    <col min="8" max="8" width="25.44140625" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
     <col min="11" max="12" width="16" customWidth="1"/>
-    <col min="16" max="16" width="28.85546875" customWidth="1"/>
-    <col min="20" max="20" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="61.85546875" customWidth="1"/>
+    <col min="16" max="16" width="28.88671875" customWidth="1"/>
+    <col min="20" max="20" width="61.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="61.88671875" customWidth="1"/>
     <col min="24" max="24" width="61" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="61" customWidth="1"/>
-    <col min="27" max="27" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="38" width="53.28515625" customWidth="1"/>
-    <col min="39" max="39" width="58.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="43" width="58.140625" customWidth="1"/>
+    <col min="27" max="27" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="38" width="53.33203125" customWidth="1"/>
+    <col min="39" max="39" width="52.21875" customWidth="1"/>
+    <col min="40" max="43" width="58.109375" customWidth="1"/>
     <col min="44" max="44" width="60" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="18.140625" customWidth="1"/>
+    <col min="45" max="45" width="18.109375" customWidth="1"/>
     <col min="47" max="47" width="16" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="54" max="57" width="9.140625" style="5"/>
-    <col min="60" max="62" width="13.85546875" customWidth="1"/>
-    <col min="63" max="63" width="35.7109375" customWidth="1"/>
-    <col min="64" max="64" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="53.5546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="57" width="9.109375" style="5"/>
+    <col min="60" max="62" width="13.88671875" customWidth="1"/>
+    <col min="63" max="63" width="35.6640625" customWidth="1"/>
+    <col min="64" max="64" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="72.5546875" customWidth="1"/>
+    <col min="66" max="66" width="11.88671875" customWidth="1"/>
+    <col min="67" max="67" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66">
+    <row r="1" spans="1:67">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1058,7 +1084,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -1073,10 +1099,10 @@
         <v>11</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>12</v>
@@ -1106,219 +1132,222 @@
         <v>20</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AU1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AY1" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="AZ1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="BA1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="BA1" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="BB1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="BC1" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="BC1" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="BD1" s="2"/>
       <c r="BE1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BF1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BG1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="BG1" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="BH1" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="BI1" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="BJ1" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="BK1" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="BL1" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="BM1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="BN1" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:66">
+        <v>151</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:67">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" t="s">
         <v>90</v>
       </c>
-      <c r="D2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>91</v>
       </c>
-      <c r="F2" t="s">
-        <v>92</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>89</v>
+        <v>203</v>
       </c>
       <c r="BB2"/>
       <c r="BC2"/>
       <c r="BD2"/>
       <c r="BE2"/>
     </row>
-    <row r="3" spans="1:66">
+    <row r="3" spans="1:67">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" t="s">
         <v>85</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>83</v>
       </c>
-      <c r="E3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="BB3"/>
       <c r="BC3"/>
       <c r="BD3"/>
       <c r="BE3"/>
     </row>
-    <row r="4" spans="1:66">
+    <row r="4" spans="1:67">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" t="s">
         <v>87</v>
       </c>
-      <c r="F4" t="s">
-        <v>88</v>
-      </c>
       <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" t="s">
         <v>33</v>
       </c>
-      <c r="I4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>34</v>
-      </c>
-      <c r="K4" t="s">
-        <v>35</v>
       </c>
       <c r="L4" t="s">
         <v>8</v>
@@ -1334,7 +1363,7 @@
       <c r="BD4"/>
       <c r="BE4"/>
     </row>
-    <row r="5" spans="1:66">
+    <row r="5" spans="1:67">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1344,13 +1373,13 @@
         <v>10</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q5" s="4">
         <v>2021</v>
       </c>
       <c r="R5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S5" s="3">
         <v>737</v>
@@ -1388,9 +1417,9 @@
       <c r="BD5"/>
       <c r="BE5"/>
     </row>
-    <row r="6" spans="1:66">
+    <row r="6" spans="1:67">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1398,13 +1427,13 @@
         <v>10</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Q6" s="4">
         <v>2021</v>
       </c>
       <c r="R6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S6" s="3">
         <v>737</v>
@@ -1442,37 +1471,37 @@
       <c r="BD6"/>
       <c r="BE6"/>
     </row>
-    <row r="7" spans="1:66">
+    <row r="7" spans="1:67">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="AQ7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AV7" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AW7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AX7" s="1" t="s">
+      <c r="AY7" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="AY7" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="BB7"/>
       <c r="BC7"/>
       <c r="BD7"/>
       <c r="BE7"/>
     </row>
-    <row r="8" spans="1:66">
+    <row r="8" spans="1:67">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
@@ -1481,22 +1510,22 @@
         <v>22</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>205</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" t="s">
         <v>39</v>
-      </c>
-      <c r="J8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" t="s">
-        <v>40</v>
       </c>
       <c r="M8">
         <v>12345</v>
@@ -1505,16 +1534,16 @@
         <v>9898989899</v>
       </c>
       <c r="AV8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AW8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AZ8">
         <v>12341</v>
       </c>
       <c r="BA8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="BB8">
         <v>5</v>
@@ -1527,9 +1556,9 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="1:66">
+    <row r="9" spans="1:67">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -1538,22 +1567,22 @@
         <v>22</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>205</v>
       </c>
       <c r="H9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" t="s">
         <v>39</v>
-      </c>
-      <c r="J9" t="s">
-        <v>41</v>
-      </c>
-      <c r="K9" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" t="s">
-        <v>40</v>
       </c>
       <c r="M9">
         <v>12345</v>
@@ -1562,16 +1591,16 @@
         <v>9898989899</v>
       </c>
       <c r="AV9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AW9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AZ9">
         <v>12341</v>
       </c>
       <c r="BA9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="BB9">
         <v>5</v>
@@ -1584,9 +1613,9 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:66">
+    <row r="10" spans="1:67">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
@@ -1595,25 +1624,25 @@
         <v>22</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>23</v>
+        <v>205</v>
       </c>
       <c r="H10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" t="s">
         <v>58</v>
       </c>
-      <c r="I10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" t="s">
-        <v>34</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>59</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="N10" s="3">
         <v>9898989899</v>
@@ -1623,27 +1652,27 @@
       <c r="BD10"/>
       <c r="BE10"/>
     </row>
-    <row r="11" spans="1:66">
+    <row r="11" spans="1:67">
       <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV11" t="s">
         <v>52</v>
-      </c>
-      <c r="AV11" t="s">
-        <v>53</v>
       </c>
       <c r="BB11"/>
       <c r="BC11"/>
       <c r="BD11"/>
       <c r="BE11"/>
     </row>
-    <row r="12" spans="1:66">
+    <row r="12" spans="1:67">
       <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
         <v>55</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>56</v>
-      </c>
-      <c r="C12" t="s">
-        <v>57</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -1653,55 +1682,55 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BB12"/>
       <c r="BC12"/>
       <c r="BD12"/>
       <c r="BE12"/>
     </row>
-    <row r="13" spans="1:66">
+    <row r="13" spans="1:67">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AV13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BB13"/>
       <c r="BC13"/>
       <c r="BD13"/>
       <c r="BE13"/>
     </row>
-    <row r="14" spans="1:66">
+    <row r="14" spans="1:67">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AV14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB14"/>
       <c r="BC14"/>
       <c r="BD14"/>
       <c r="BE14"/>
     </row>
-    <row r="15" spans="1:66">
+    <row r="15" spans="1:67">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AV15" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BB15"/>
       <c r="BC15"/>
       <c r="BD15"/>
       <c r="BE15"/>
     </row>
-    <row r="16" spans="1:66">
+    <row r="16" spans="1:67">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AV16" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BB16"/>
       <c r="BC16"/>
@@ -1710,99 +1739,99 @@
     </row>
     <row r="17" spans="1:66">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>23</v>
+        <v>205</v>
       </c>
       <c r="BB17"/>
       <c r="BC17"/>
       <c r="BD17"/>
       <c r="BE17"/>
       <c r="BF17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="BG17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:66">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BB18"/>
       <c r="BC18"/>
       <c r="BD18"/>
       <c r="BE18"/>
       <c r="BM18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:66">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="BB19"/>
       <c r="BC19"/>
       <c r="BD19"/>
       <c r="BE19"/>
       <c r="BM19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:66">
       <c r="A20" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV20" t="s">
         <v>80</v>
-      </c>
-      <c r="AV20" t="s">
-        <v>81</v>
       </c>
       <c r="BB20"/>
       <c r="BC20"/>
       <c r="BD20"/>
       <c r="BE20"/>
       <c r="BN20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:66">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
         <v>89</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>90</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>91</v>
       </c>
-      <c r="F21" t="s">
-        <v>92</v>
-      </c>
       <c r="G21" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:66">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P22" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q22" s="7">
         <v>2030</v>
       </c>
       <c r="R22" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
@@ -1831,34 +1860,34 @@
       <c r="AR22" s="7"/>
       <c r="AS22" s="7"/>
       <c r="AT22" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AU22" s="7"/>
     </row>
     <row r="23" spans="1:66">
       <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" t="s">
         <v>101</v>
       </c>
-      <c r="E23" t="s">
-        <v>103</v>
-      </c>
       <c r="F23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>102</v>
+        <v>205</v>
       </c>
       <c r="H23" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" t="s">
         <v>58</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>59</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="N23" s="3">
         <v>9898989899</v>
@@ -1866,23 +1895,23 @@
     </row>
     <row r="24" spans="1:66">
       <c r="A24" t="s">
+        <v>194</v>
+      </c>
+      <c r="E24" t="s">
+        <v>195</v>
+      </c>
+      <c r="F24" t="s">
         <v>196</v>
-      </c>
-      <c r="E24" t="s">
-        <v>197</v>
-      </c>
-      <c r="F24" t="s">
-        <v>198</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
+        <v>197</v>
+      </c>
+      <c r="K24" t="s">
+        <v>198</v>
+      </c>
+      <c r="M24" s="7" t="s">
         <v>199</v>
-      </c>
-      <c r="K24" t="s">
-        <v>200</v>
-      </c>
-      <c r="M24" s="7" t="s">
-        <v>201</v>
       </c>
       <c r="N24" s="3">
         <v>9898989899</v>
@@ -1893,240 +1922,240 @@
         <v>6</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:66">
       <c r="A26" t="s">
+        <v>104</v>
+      </c>
+      <c r="BL26" t="s">
         <v>106</v>
       </c>
-      <c r="BL26" t="s">
+    </row>
+    <row r="27" spans="1:66" ht="57.6">
+      <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="BK27" s="10" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:66" ht="60">
-      <c r="A27" t="s">
-        <v>109</v>
-      </c>
-      <c r="BK27" s="10" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:66">
       <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="BH28" s="11" t="s">
         <v>112</v>
-      </c>
-      <c r="BH28" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="BI28" s="11"/>
       <c r="BJ28" s="11"/>
     </row>
     <row r="29" spans="1:66">
       <c r="A29" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS29" t="s">
         <v>115</v>
-      </c>
-      <c r="AS29" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:66">
       <c r="A30" t="s">
+        <v>116</v>
+      </c>
+      <c r="BJ30" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="BJ30" s="11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:66">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="BI31" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:66">
       <c r="A32" t="s">
+        <v>121</v>
+      </c>
+      <c r="AR32" t="s">
         <v>123</v>
-      </c>
-      <c r="AR32" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:41">
       <c r="A33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AA33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:41">
       <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA34" t="s">
         <v>52</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:41">
       <c r="A35" t="s">
+        <v>126</v>
+      </c>
+      <c r="X35" t="s">
         <v>128</v>
-      </c>
-      <c r="X35" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:41">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="T36" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="U36" s="13"/>
       <c r="V36" s="13"/>
       <c r="W36" s="13"/>
       <c r="AD36" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:41">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:41">
       <c r="A38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AB38" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AC38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AE38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AG38" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AH38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AI38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AJ38" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AK38" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="AM38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:41">
       <c r="A39" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y39" t="s">
         <v>149</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:41">
       <c r="A40" t="s">
+        <v>154</v>
+      </c>
+      <c r="AL40" t="s">
         <v>156</v>
-      </c>
-      <c r="AL40" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:41">
       <c r="A41" t="s">
+        <v>157</v>
+      </c>
+      <c r="AO41" t="s">
         <v>159</v>
-      </c>
-      <c r="AO41" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:41">
       <c r="A42" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AF42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:41">
       <c r="A43" t="s">
+        <v>164</v>
+      </c>
+      <c r="U43" t="s">
         <v>166</v>
-      </c>
-      <c r="U43" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:41">
       <c r="A44" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="D44" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E44" t="s">
         <v>174</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="F44" t="s">
         <v>175</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E44" t="s">
-        <v>176</v>
-      </c>
-      <c r="F44" t="s">
-        <v>177</v>
-      </c>
       <c r="G44" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:41">
       <c r="A45" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:41">
       <c r="A46" t="s">
+        <v>177</v>
+      </c>
+      <c r="E46" t="s">
+        <v>178</v>
+      </c>
+      <c r="F46" t="s">
         <v>179</v>
       </c>
-      <c r="E46" t="s">
+      <c r="G46" t="s">
         <v>180</v>
       </c>
-      <c r="F46" t="s">
-        <v>181</v>
-      </c>
-      <c r="G46" t="s">
-        <v>182</v>
-      </c>
       <c r="H46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M46">
         <v>12345</v>
@@ -2137,63 +2166,96 @@
     </row>
     <row r="47" spans="1:41">
       <c r="A47" t="s">
+        <v>185</v>
+      </c>
+      <c r="V47" t="s">
         <v>187</v>
-      </c>
-      <c r="V47" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:41">
       <c r="A48" t="s">
+        <v>188</v>
+      </c>
+      <c r="AN48" t="s">
         <v>190</v>
       </c>
-      <c r="AN48" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26">
+    </row>
+    <row r="49" spans="1:67">
       <c r="A49" t="s">
+        <v>191</v>
+      </c>
+      <c r="W49" t="s">
         <v>193</v>
       </c>
-      <c r="W49" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="50" spans="1:26">
+    </row>
+    <row r="50" spans="1:67">
       <c r="A50" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z50" t="s">
         <v>202</v>
       </c>
-      <c r="Z50" t="s">
-        <v>204</v>
+    </row>
+    <row r="51" spans="1:67">
+      <c r="A51" t="s">
+        <v>206</v>
+      </c>
+      <c r="BO51" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="1:67">
+      <c r="A52" t="s">
+        <v>209</v>
+      </c>
+      <c r="P52" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q52" s="7">
+        <v>2030</v>
+      </c>
+      <c r="R52" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="S52" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:67">
+      <c r="A53" t="s">
+        <v>211</v>
+      </c>
+      <c r="C53" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Vihaan@2018" xr:uid="{4F5DD53B-FDBE-495F-B268-88C5E8B1BE36}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{4B3C725C-3736-453A-973F-014EA407F106}"/>
-    <hyperlink ref="AX7" r:id="rId3" xr:uid="{72305042-87C7-4932-8AE0-68B10841BE88}"/>
-    <hyperlink ref="AY7" r:id="rId4" xr:uid="{475D0090-7A14-45A1-B12D-CC9A2AB68BA3}"/>
-    <hyperlink ref="G8" r:id="rId5" xr:uid="{01FC8DE1-D0EC-434A-A443-9B88FB015484}"/>
-    <hyperlink ref="G9" r:id="rId6" xr:uid="{7F86A831-6BAE-4F74-AB10-D461CC901815}"/>
-    <hyperlink ref="G10" r:id="rId7" xr:uid="{F135D05F-7B8D-4589-985B-77D2AC13D428}"/>
-    <hyperlink ref="G3" r:id="rId8" xr:uid="{42EA2C65-3A92-42BA-B87A-FAAA8E7932EF}"/>
-    <hyperlink ref="G17" r:id="rId9" xr:uid="{B5A52BEE-BD07-4192-8B79-0E8862B00DAB}"/>
-    <hyperlink ref="C3" r:id="rId10" xr:uid="{5C93EFB9-4664-4EA0-A86E-6CA8D6CECDB7}"/>
-    <hyperlink ref="B3" r:id="rId11" xr:uid="{65DA951E-3E12-41E2-9629-FC7DCE875142}"/>
-    <hyperlink ref="G2" r:id="rId12" xr:uid="{10DB1590-259A-461C-BAB1-C7EFA3720336}"/>
-    <hyperlink ref="G21" r:id="rId13" xr:uid="{E0346E4E-E05A-47AD-8F33-01EBB09E6BA1}"/>
-    <hyperlink ref="B21" r:id="rId14" xr:uid="{65842A3E-E6DD-4D79-A78A-D8E6C5FD69F0}"/>
-    <hyperlink ref="C21" r:id="rId15" display="Vihaan@2018" xr:uid="{F0F6AA98-A15F-47FF-89C8-53113FA25486}"/>
-    <hyperlink ref="D2" r:id="rId16" display="Vihaan@2018" xr:uid="{5C518423-99A0-4586-B3F5-D544A737B8F9}"/>
-    <hyperlink ref="G23" r:id="rId17" xr:uid="{1271EC5C-450C-4B58-9AE6-69B21901206E}"/>
-    <hyperlink ref="G25" r:id="rId18" xr:uid="{4C9855DC-6136-4EC1-B891-FB67685B8484}"/>
-    <hyperlink ref="B44" r:id="rId19" xr:uid="{E6B3FA17-5B57-4416-BDD3-91CF4EEC85D0}"/>
-    <hyperlink ref="C44" r:id="rId20" xr:uid="{E64F5A25-4DA8-46BD-838F-574B6DB05927}"/>
-    <hyperlink ref="D44" r:id="rId21" xr:uid="{C9748A95-B1CA-47DF-AA51-00A799A5CA31}"/>
-    <hyperlink ref="B45" r:id="rId22" xr:uid="{1E3AF817-4B8E-42D4-8F7B-0BCE2E35316F}"/>
-    <hyperlink ref="C45" r:id="rId23" xr:uid="{03AE5693-B809-440D-AFF6-4E56A33D210F}"/>
-    <hyperlink ref="G44" r:id="rId24" xr:uid="{B7F7FE31-A565-423F-9484-A0BBD29B1DAE}"/>
-    <hyperlink ref="G45" r:id="rId25" xr:uid="{8743381F-49E5-42D0-846F-4FD5EA879AED}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{4F5DD53B-FDBE-495F-B268-88C5E8B1BE36}"/>
+    <hyperlink ref="AX7" r:id="rId2" xr:uid="{72305042-87C7-4932-8AE0-68B10841BE88}"/>
+    <hyperlink ref="AY7" r:id="rId3" xr:uid="{475D0090-7A14-45A1-B12D-CC9A2AB68BA3}"/>
+    <hyperlink ref="G8" r:id="rId4" display="harish.chiruvella1@gmail.com" xr:uid="{01FC8DE1-D0EC-434A-A443-9B88FB015484}"/>
+    <hyperlink ref="G9" r:id="rId5" display="harish.chiruvella1@gmail.com" xr:uid="{7F86A831-6BAE-4F74-AB10-D461CC901815}"/>
+    <hyperlink ref="G10" r:id="rId6" display="harish.chiruvella1@gmail.com" xr:uid="{F135D05F-7B8D-4589-985B-77D2AC13D428}"/>
+    <hyperlink ref="G3" r:id="rId7" xr:uid="{42EA2C65-3A92-42BA-B87A-FAAA8E7932EF}"/>
+    <hyperlink ref="G17" r:id="rId8" display="harish.chiruvella1@gmail.com" xr:uid="{B5A52BEE-BD07-4192-8B79-0E8862B00DAB}"/>
+    <hyperlink ref="C3" r:id="rId9" xr:uid="{5C93EFB9-4664-4EA0-A86E-6CA8D6CECDB7}"/>
+    <hyperlink ref="B3" r:id="rId10" xr:uid="{65DA951E-3E12-41E2-9629-FC7DCE875142}"/>
+    <hyperlink ref="G21" r:id="rId11" xr:uid="{E0346E4E-E05A-47AD-8F33-01EBB09E6BA1}"/>
+    <hyperlink ref="B21" r:id="rId12" xr:uid="{65842A3E-E6DD-4D79-A78A-D8E6C5FD69F0}"/>
+    <hyperlink ref="C21" r:id="rId13" display="Vihaan@2018" xr:uid="{F0F6AA98-A15F-47FF-89C8-53113FA25486}"/>
+    <hyperlink ref="G23" r:id="rId14" xr:uid="{1271EC5C-450C-4B58-9AE6-69B21901206E}"/>
+    <hyperlink ref="G25" r:id="rId15" xr:uid="{4C9855DC-6136-4EC1-B891-FB67685B8484}"/>
+    <hyperlink ref="B44" r:id="rId16" xr:uid="{E6B3FA17-5B57-4416-BDD3-91CF4EEC85D0}"/>
+    <hyperlink ref="C44" r:id="rId17" xr:uid="{E64F5A25-4DA8-46BD-838F-574B6DB05927}"/>
+    <hyperlink ref="D44" r:id="rId18" xr:uid="{C9748A95-B1CA-47DF-AA51-00A799A5CA31}"/>
+    <hyperlink ref="B45" r:id="rId19" xr:uid="{1E3AF817-4B8E-42D4-8F7B-0BCE2E35316F}"/>
+    <hyperlink ref="C45" r:id="rId20" xr:uid="{03AE5693-B809-440D-AFF6-4E56A33D210F}"/>
+    <hyperlink ref="G44" r:id="rId21" xr:uid="{B7F7FE31-A565-423F-9484-A0BBD29B1DAE}"/>
+    <hyperlink ref="G45" r:id="rId22" xr:uid="{8743381F-49E5-42D0-846F-4FD5EA879AED}"/>
+    <hyperlink ref="B2" r:id="rId23" xr:uid="{7C9C7214-237B-4CF0-8FDF-478AE4FD7575}"/>
+    <hyperlink ref="D2" r:id="rId24" xr:uid="{BD721168-2425-4853-B0B1-63E48A0519F9}"/>
+    <hyperlink ref="G2" r:id="rId25" xr:uid="{94048FE4-BA3B-4D90-817F-B540AFE54434}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId26"/>

</xml_diff>